<commit_message>
add necessary GUI widgets, first picture!
</commit_message>
<xml_diff>
--- a/data_test.xlsx
+++ b/data_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="bg" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t xml:space="preserve">image</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">rotate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1.bmp</t>
   </si>
   <si>
     <t xml:space="preserve">BORDER</t>
@@ -160,15 +163,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,89 +194,103 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="n">
+      <c r="E1" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F1" s="0" t="n">
+      <c r="F1" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="2" t="n">
         <v>140</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>140</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -298,121 +315,121 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="2" t="n">
         <v>130</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>140</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>44740.5</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <v>0.93</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="2" t="n">
         <v>0.8</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="2" t="n">
         <v>400</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="2" t="n">
         <v>700</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="2" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>44740</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>0.93</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="2" t="n">
         <v>400</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="2" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>44740</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
         <v>0.93</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="2" t="n">
         <v>700</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="2" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H10" s="4"/>
+      <c r="H10" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -436,56 +453,56 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>11</v>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="2" t="n">
         <v>140</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>140</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>44740</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="2" t="n">
         <v>140</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>140</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>44740</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -505,71 +522,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T30" activeCellId="0" sqref="T30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44740</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44740</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>44740</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>44740</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>